<commit_message>
-Update the GNSS Module (SAM-M10Q-00B) in BOM and Schematic files
</commit_message>
<xml_diff>
--- a/H1FR50/Released/BOM/H1FR50.xlsx
+++ b/H1FR50/Released/BOM/H1FR50.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\OneDrive\Documents\H1FR5x-Hardware\H1FR50\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Documents\H1FR5x-Hardware\H1FR50\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D478571-0358-48DB-8BA7-8CC703691FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54EE15A-56D1-4F84-A534-761373ADB39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,18 +274,9 @@
     <t>U2</t>
   </si>
   <si>
-    <t>SAM-M8Q-0-10</t>
-  </si>
-  <si>
     <t>u-blox</t>
   </si>
   <si>
-    <t>https://octopart.com/sam-m8q-0-10-u-blox-88247750?r=sp</t>
-  </si>
-  <si>
-    <t>RF RX GALILEO 1.575GHZ/1.602GHZ</t>
-  </si>
-  <si>
     <t>R1 , R4 , R5 , R6 , R7</t>
   </si>
   <si>
@@ -302,6 +293,15 @@
   </si>
   <si>
     <t>https://octopart.com/crcw0603150rfkea-vishay-39455211?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/sam-m10q-00b-u-blox-130040883?r=sp</t>
+  </si>
+  <si>
+    <t>SAM-M10Q-00B</t>
+  </si>
+  <si>
+    <t>u-blox M10 GNSS antenna module ROM, TCXO, SAW, LNA LGA</t>
   </si>
 </sst>
 </file>
@@ -312,7 +312,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -320,7 +320,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -331,21 +331,21 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -358,7 +358,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -379,7 +379,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -404,7 +404,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -553,32 +552,32 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -957,22 +956,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="70.59765625" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
@@ -984,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -993,7 +992,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1003,14 +1002,14 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="20">
         <v>0</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1020,29 +1019,29 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>44815</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>21</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>26</v>
       </c>
@@ -1102,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>70</v>
       </c>
@@ -1122,27 +1121,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>90</v>
-      </c>
       <c r="C12" s="15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F12" s="17">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
@@ -1162,9 +1161,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>66</v>
@@ -1182,7 +1181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>72</v>
       </c>
@@ -1202,7 +1201,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>73</v>
       </c>
@@ -1222,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>74</v>
       </c>
@@ -1242,7 +1241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>43</v>
       </c>
@@ -1262,7 +1261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>75</v>
       </c>
@@ -1282,7 +1281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>80</v>
       </c>
@@ -1302,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>79</v>
       </c>
@@ -1322,7 +1321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>53</v>
       </c>
@@ -1342,27 +1341,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
         <v>81</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C23" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>84</v>
+      <c r="E23" s="19" t="s">
+        <v>89</v>
       </c>
       <c r="F23" s="17">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>59</v>
       </c>
@@ -1402,10 +1401,9 @@
     <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="E21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E23" r:id="rId14" xr:uid="{E79E2485-7F6C-418F-8EA8-F53E7A084965}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>